<commit_message>
PAMS (1).txt erstellt. Bilder eingefügt
</commit_message>
<xml_diff>
--- a/documents/projectmanagement/3_Planung/Gantt_Projektplan.xlsx
+++ b/documents/projectmanagement/3_Planung/Gantt_Projektplan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11592"/>
   </bookViews>
   <sheets>
     <sheet name="Projekt" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
   <si>
     <t>Projektplanung</t>
   </si>
@@ -59,84 +59,6 @@
   </si>
   <si>
     <t>AKTIVITÄT</t>
-  </si>
-  <si>
-    <t>Aktivität 01</t>
-  </si>
-  <si>
-    <t>Aktivität 02</t>
-  </si>
-  <si>
-    <t>Aktivität 03</t>
-  </si>
-  <si>
-    <t>Aktivität 04</t>
-  </si>
-  <si>
-    <t>Aktivität 05</t>
-  </si>
-  <si>
-    <t>Aktivität 06</t>
-  </si>
-  <si>
-    <t>Aktivität 07</t>
-  </si>
-  <si>
-    <t>Aktivität 08</t>
-  </si>
-  <si>
-    <t>Aktivität 09</t>
-  </si>
-  <si>
-    <t>Aktivität 10</t>
-  </si>
-  <si>
-    <t>Aktivität 11</t>
-  </si>
-  <si>
-    <t>Aktivität 12</t>
-  </si>
-  <si>
-    <t>Aktivität 13</t>
-  </si>
-  <si>
-    <t>Aktivität 14</t>
-  </si>
-  <si>
-    <t>Aktivität 15</t>
-  </si>
-  <si>
-    <t>Aktivität 16</t>
-  </si>
-  <si>
-    <t>Aktivität 17</t>
-  </si>
-  <si>
-    <t>Aktivität 18</t>
-  </si>
-  <si>
-    <t>Aktivität 19</t>
-  </si>
-  <si>
-    <t>Aktivität 20</t>
-  </si>
-  <si>
-    <t>Aktivität 21</t>
-  </si>
-  <si>
-    <t>Aktivität 22</t>
-  </si>
-  <si>
-    <t>Aktivität 23</t>
-  </si>
-  <si>
-    <t>Aktivität 24</t>
-  </si>
-  <si>
-    <t>Aktivität 25</t>
-  </si>
-  <si>
-    <t>Aktivität 26</t>
   </si>
   <si>
     <r>
@@ -207,12 +129,138 @@
   <si>
     <t>Tage</t>
   </si>
+  <si>
+    <t>Projektstart</t>
+  </si>
+  <si>
+    <t>Zieldefinition erstellen</t>
+  </si>
+  <si>
+    <t>Projekt-Initialisierung</t>
+  </si>
+  <si>
+    <t>Projektsteckbrief</t>
+  </si>
+  <si>
+    <t>Umfeldanalyse</t>
+  </si>
+  <si>
+    <t>Chancen und Risiko-Portfolio</t>
+  </si>
+  <si>
+    <t>Dokumentationsrichtlinien</t>
+  </si>
+  <si>
+    <t>Coding-Guidelines</t>
+  </si>
+  <si>
+    <t>Unternehmensstrukturanalyse</t>
+  </si>
+  <si>
+    <t>Machbarkeitsstudie erstellen</t>
+  </si>
+  <si>
+    <t>Projekt-Definition</t>
+  </si>
+  <si>
+    <t>Pflichtenheft erstellen</t>
+  </si>
+  <si>
+    <t>Projektauftrag erstellen</t>
+  </si>
+  <si>
+    <t>Kalkulation der Projektkosten</t>
+  </si>
+  <si>
+    <t>Kommunikationsstrategie</t>
+  </si>
+  <si>
+    <t>Risikoanalyse</t>
+  </si>
+  <si>
+    <t>Kennzahlenmodell erstellen</t>
+  </si>
+  <si>
+    <t>Kick-Off-Meeting</t>
+  </si>
+  <si>
+    <t>Projektantrag unterschreiben</t>
+  </si>
+  <si>
+    <t>Konzeption</t>
+  </si>
+  <si>
+    <t>Systemübersicht erstellen</t>
+  </si>
+  <si>
+    <t>Use-Cases definieren</t>
+  </si>
+  <si>
+    <t>Berechtigungskonzept erstellen</t>
+  </si>
+  <si>
+    <t>EPK modellieren</t>
+  </si>
+  <si>
+    <t>ERM modellieren</t>
+  </si>
+  <si>
+    <t>Mockups erstellen</t>
+  </si>
+  <si>
+    <t>Implementierung</t>
+  </si>
+  <si>
+    <t>Programmierung SQL</t>
+  </si>
+  <si>
+    <t>Programmierung PHP</t>
+  </si>
+  <si>
+    <t>Programmierung Javascript</t>
+  </si>
+  <si>
+    <t>Programmierung HTML</t>
+  </si>
+  <si>
+    <t>Programmierung CSS</t>
+  </si>
+  <si>
+    <t>Projektkontrolle</t>
+  </si>
+  <si>
+    <t>Kontrolle der Kennzahlen</t>
+  </si>
+  <si>
+    <t>Qualitätssicherungsmaßnahmen bestimmen</t>
+  </si>
+  <si>
+    <t>Projektabschluss</t>
+  </si>
+  <si>
+    <t>Produktabnahme</t>
+  </si>
+  <si>
+    <t>Projektabschlussanalyse</t>
+  </si>
+  <si>
+    <t>Erfahrungssicherung</t>
+  </si>
+  <si>
+    <t>Projektauflösung</t>
+  </si>
+  <si>
+    <t>Test Blackbox</t>
+  </si>
+  <si>
+    <t>Test Whitebox</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -242,12 +290,6 @@
       <name val="Corbel"/>
       <family val="2"/>
       <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="1" tint="0.24994659260841701"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <sz val="12"/>
@@ -291,11 +333,26 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <b/>
+      <sz val="8"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color theme="7"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -389,14 +446,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="3" applyFill="0" applyProtection="0">
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="3" applyFill="0" applyProtection="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
@@ -405,11 +462,11 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -419,13 +476,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="3" xfId="3">
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="3" xfId="3">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1">
@@ -434,7 +491,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="6">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="7">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="7">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -452,25 +509,28 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="6" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="7" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="7" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -650,7 +710,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="Ausgewählter_Zeitraum" max="60" min="1" page="10" val="8"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="Ausgewählter_Zeitraum" max="60" min="1" page="10"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -660,15 +720,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>17</xdr:col>
-          <xdr:colOff>66675</xdr:colOff>
+          <xdr:colOff>68580</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>30480</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>17</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:col>18</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>257175</xdr:rowOff>
+          <xdr:rowOff>259080</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -935,44 +995,44 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:BQ34"/>
+  <dimension ref="B2:BD50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.77734375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.625" customWidth="1"/>
-    <col min="2" max="2" width="15.875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.25" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.25" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="7.25" style="7" customWidth="1"/>
-    <col min="8" max="8" width="4.25" style="1" customWidth="1"/>
-    <col min="9" max="28" width="2.75" style="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="35.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.21875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="7.21875" style="7" customWidth="1"/>
+    <col min="8" max="8" width="4.21875" style="1" customWidth="1"/>
+    <col min="9" max="28" width="2.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:69" ht="15" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-    </row>
-    <row r="3" spans="2:69" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="I3" s="8" t="s">
-        <v>38</v>
+    <row r="2" spans="2:56" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B2" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+    </row>
+    <row r="3" spans="2:56" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="I3" s="19" t="s">
+        <v>12</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
@@ -981,28 +1041,28 @@
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
       <c r="P3" s="8"/>
-      <c r="Q3" s="19">
-        <v>8</v>
+      <c r="Q3" s="20">
+        <v>1</v>
       </c>
       <c r="R3" s="8"/>
       <c r="T3" s="9"/>
-      <c r="U3" s="18" t="s">
+      <c r="U3" s="17" t="s">
         <v>1</v>
       </c>
       <c r="X3" s="10"/>
-      <c r="Y3" s="18" t="s">
+      <c r="Y3" s="17" t="s">
         <v>2</v>
       </c>
       <c r="AA3" s="11"/>
       <c r="AB3" s="6" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
       <c r="AE3" s="1"/>
       <c r="AF3" s="12"/>
-      <c r="AG3" s="18" t="s">
-        <v>39</v>
+      <c r="AG3" s="17" t="s">
+        <v>13</v>
       </c>
       <c r="AJ3" s="1"/>
       <c r="AK3" s="1"/>
@@ -1010,28 +1070,28 @@
       <c r="AM3" s="1"/>
       <c r="AP3" s="13"/>
       <c r="AQ3" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
       <c r="AT4" s="1"/>
       <c r="AU4" s="1"/>
       <c r="AV4" s="1"/>
       <c r="AW4" s="1"/>
       <c r="AX4" s="1"/>
     </row>
-    <row r="5" spans="2:69" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:56" x14ac:dyDescent="0.35">
       <c r="AT5" s="1"/>
       <c r="AU5" s="1"/>
       <c r="AV5" s="1"/>
     </row>
-    <row r="6" spans="2:69" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:56" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
         <v>3</v>
@@ -1055,7 +1115,7 @@
       <c r="AU6" s="1"/>
       <c r="AV6" s="1"/>
     </row>
-    <row r="7" spans="2:69" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:56" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1076,11 +1136,11 @@
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="2:69" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:56" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -1229,572 +1289,715 @@
       <c r="BC8" s="3">
         <v>47</v>
       </c>
-      <c r="BD8" s="3">
+      <c r="BD8" s="1"/>
+    </row>
+    <row r="9" spans="2:56" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="14">
+        <v>1</v>
+      </c>
+      <c r="D9" s="14">
+        <v>1</v>
+      </c>
+      <c r="E9" s="14">
+        <v>1</v>
+      </c>
+      <c r="F9" s="14">
+        <v>1</v>
+      </c>
+      <c r="G9" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="14">
+        <v>1</v>
+      </c>
+      <c r="D10" s="14">
+        <v>6</v>
+      </c>
+      <c r="E10" s="14">
+        <v>1</v>
+      </c>
+      <c r="F10" s="14">
+        <v>6</v>
+      </c>
+      <c r="G10" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:56" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="14">
+        <v>3</v>
+      </c>
+      <c r="D11" s="14">
+        <v>4</v>
+      </c>
+      <c r="E11" s="14">
+        <v>3</v>
+      </c>
+      <c r="F11" s="14">
+        <v>5</v>
+      </c>
+      <c r="G11" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:56" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="14">
+        <v>4</v>
+      </c>
+      <c r="D12" s="14">
+        <v>8</v>
+      </c>
+      <c r="E12" s="14">
+        <v>4</v>
+      </c>
+      <c r="F12" s="14">
+        <v>6</v>
+      </c>
+      <c r="G12" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:56" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="14">
+        <v>4</v>
+      </c>
+      <c r="D13" s="14">
+        <v>2</v>
+      </c>
+      <c r="E13" s="14">
+        <v>4</v>
+      </c>
+      <c r="F13" s="14">
+        <v>8</v>
+      </c>
+      <c r="G13" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:56" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="14">
+        <v>4</v>
+      </c>
+      <c r="D14" s="14">
+        <v>3</v>
+      </c>
+      <c r="E14" s="14">
+        <v>4</v>
+      </c>
+      <c r="F14" s="14">
+        <v>6</v>
+      </c>
+      <c r="G14" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:56" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="14">
+        <v>5</v>
+      </c>
+      <c r="D15" s="14">
+        <v>4</v>
+      </c>
+      <c r="E15" s="14">
+        <v>5</v>
+      </c>
+      <c r="F15" s="14">
+        <v>3</v>
+      </c>
+      <c r="G15" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:56" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="14">
+        <v>5</v>
+      </c>
+      <c r="D17" s="14">
+        <v>2</v>
+      </c>
+      <c r="E17" s="14">
+        <v>5</v>
+      </c>
+      <c r="F17" s="14">
+        <v>5</v>
+      </c>
+      <c r="G17" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="14">
+        <v>5</v>
+      </c>
+      <c r="D18" s="14">
+        <v>2</v>
+      </c>
+      <c r="E18" s="14">
+        <v>5</v>
+      </c>
+      <c r="F18" s="14">
+        <v>6</v>
+      </c>
+      <c r="G18" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="14">
+        <v>6</v>
+      </c>
+      <c r="D19" s="14">
+        <v>5</v>
+      </c>
+      <c r="E19" s="14">
+        <v>6</v>
+      </c>
+      <c r="F19" s="14">
+        <v>7</v>
+      </c>
+      <c r="G19" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="16">
+        <v>6</v>
+      </c>
+      <c r="D20" s="14">
+        <v>1</v>
+      </c>
+      <c r="E20" s="14">
+        <v>5</v>
+      </c>
+      <c r="F20" s="14">
+        <v>8</v>
+      </c>
+      <c r="G20" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="14">
+        <v>9</v>
+      </c>
+      <c r="D21" s="14">
+        <v>3</v>
+      </c>
+      <c r="E21" s="14">
+        <v>9</v>
+      </c>
+      <c r="F21" s="14">
+        <v>3</v>
+      </c>
+      <c r="G21" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="14">
+        <v>9</v>
+      </c>
+      <c r="D22" s="14">
+        <v>6</v>
+      </c>
+      <c r="E22" s="14">
+        <v>9</v>
+      </c>
+      <c r="F22" s="14">
+        <v>7</v>
+      </c>
+      <c r="G22" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="14">
+        <v>9</v>
+      </c>
+      <c r="D23" s="14">
+        <v>3</v>
+      </c>
+      <c r="E23" s="14">
+        <v>9</v>
+      </c>
+      <c r="F23" s="14">
+        <v>1</v>
+      </c>
+      <c r="G23" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="14">
+        <v>9</v>
+      </c>
+      <c r="D24" s="14">
+        <v>4</v>
+      </c>
+      <c r="E24" s="14">
+        <v>8</v>
+      </c>
+      <c r="F24" s="14">
+        <v>5</v>
+      </c>
+      <c r="G24" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="14">
+        <v>10</v>
+      </c>
+      <c r="D25" s="14">
+        <v>5</v>
+      </c>
+      <c r="E25" s="14">
+        <v>10</v>
+      </c>
+      <c r="F25" s="14">
+        <v>3</v>
+      </c>
+      <c r="G25" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="14">
+        <v>11</v>
+      </c>
+      <c r="D26" s="14">
+        <v>2</v>
+      </c>
+      <c r="E26" s="14">
+        <v>11</v>
+      </c>
+      <c r="F26" s="14">
+        <v>5</v>
+      </c>
+      <c r="G26" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="14">
+        <v>12</v>
+      </c>
+      <c r="D27" s="14">
+        <v>6</v>
+      </c>
+      <c r="E27" s="14">
+        <v>12</v>
+      </c>
+      <c r="F27" s="14">
+        <v>7</v>
+      </c>
+      <c r="G27" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="14">
+        <v>12</v>
+      </c>
+      <c r="D28" s="14">
+        <v>1</v>
+      </c>
+      <c r="E28" s="14">
+        <v>12</v>
+      </c>
+      <c r="F28" s="14">
+        <v>5</v>
+      </c>
+      <c r="G28" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="14">
+        <v>14</v>
+      </c>
+      <c r="D29" s="14">
+        <v>5</v>
+      </c>
+      <c r="E29" s="14">
+        <v>14</v>
+      </c>
+      <c r="F29" s="14">
+        <v>6</v>
+      </c>
+      <c r="G29" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="14">
+        <v>14</v>
+      </c>
+      <c r="D30" s="14">
+        <v>8</v>
+      </c>
+      <c r="E30" s="14">
+        <v>14</v>
+      </c>
+      <c r="F30" s="14">
+        <v>2</v>
+      </c>
+      <c r="G30" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="14">
+        <v>14</v>
+      </c>
+      <c r="D41" s="14">
+        <v>7</v>
+      </c>
+      <c r="E41" s="14">
+        <v>14</v>
+      </c>
+      <c r="F41" s="14">
+        <v>3</v>
+      </c>
+      <c r="G41" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" s="14">
+        <v>15</v>
+      </c>
+      <c r="D42" s="14">
+        <v>4</v>
+      </c>
+      <c r="E42" s="14">
+        <v>15</v>
+      </c>
+      <c r="F42" s="14">
+        <v>8</v>
+      </c>
+      <c r="G42" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" s="14">
+        <v>15</v>
+      </c>
+      <c r="D43" s="14">
+        <v>5</v>
+      </c>
+      <c r="E43" s="14">
+        <v>15</v>
+      </c>
+      <c r="F43" s="14">
+        <v>3</v>
+      </c>
+      <c r="G43" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="15"/>
+    </row>
+    <row r="45" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="BE8" s="3">
-        <v>49</v>
-      </c>
-      <c r="BF8" s="3">
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="BG8" s="3">
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="BH8" s="3">
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="BI8" s="3">
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="BJ8" s="3">
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B50" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="BK8" s="3">
-        <v>55</v>
-      </c>
-      <c r="BL8" s="3">
-        <v>56</v>
-      </c>
-      <c r="BM8" s="3">
-        <v>57</v>
-      </c>
-      <c r="BN8" s="3">
-        <v>58</v>
-      </c>
-      <c r="BO8" s="3">
-        <v>59</v>
-      </c>
-      <c r="BP8" s="3">
-        <v>60</v>
-      </c>
-      <c r="BQ8" s="1"/>
-    </row>
-    <row r="9" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="15">
-        <v>1</v>
-      </c>
-      <c r="D9" s="15">
-        <v>5</v>
-      </c>
-      <c r="E9" s="15">
-        <v>1</v>
-      </c>
-      <c r="F9" s="15">
-        <v>4</v>
-      </c>
-      <c r="G9" s="16">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="10" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="15">
-        <v>1</v>
-      </c>
-      <c r="D10" s="15">
-        <v>6</v>
-      </c>
-      <c r="E10" s="15">
-        <v>1</v>
-      </c>
-      <c r="F10" s="15">
-        <v>6</v>
-      </c>
-      <c r="G10" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="15">
-        <v>2</v>
-      </c>
-      <c r="D11" s="15">
-        <v>4</v>
-      </c>
-      <c r="E11" s="15">
-        <v>2</v>
-      </c>
-      <c r="F11" s="15">
-        <v>5</v>
-      </c>
-      <c r="G11" s="16">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="12" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="15">
-        <v>4</v>
-      </c>
-      <c r="D12" s="15">
-        <v>8</v>
-      </c>
-      <c r="E12" s="15">
-        <v>4</v>
-      </c>
-      <c r="F12" s="15">
-        <v>6</v>
-      </c>
-      <c r="G12" s="16">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="15">
-        <v>4</v>
-      </c>
-      <c r="D13" s="15">
-        <v>2</v>
-      </c>
-      <c r="E13" s="15">
-        <v>4</v>
-      </c>
-      <c r="F13" s="15">
-        <v>8</v>
-      </c>
-      <c r="G13" s="16">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="14" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="15">
-        <v>4</v>
-      </c>
-      <c r="D14" s="15">
-        <v>3</v>
-      </c>
-      <c r="E14" s="15">
-        <v>4</v>
-      </c>
-      <c r="F14" s="15">
-        <v>6</v>
-      </c>
-      <c r="G14" s="16">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="15" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="14" t="s">
+      <c r="C50" s="14">
         <v>16</v>
       </c>
-      <c r="C15" s="15">
-        <v>5</v>
-      </c>
-      <c r="D15" s="15">
-        <v>4</v>
-      </c>
-      <c r="E15" s="15">
-        <v>5</v>
-      </c>
-      <c r="F15" s="15">
-        <v>3</v>
-      </c>
-      <c r="G15" s="16">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="16" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="15">
-        <v>5</v>
-      </c>
-      <c r="D16" s="15">
-        <v>2</v>
-      </c>
-      <c r="E16" s="15">
-        <v>5</v>
-      </c>
-      <c r="F16" s="15">
-        <v>5</v>
-      </c>
-      <c r="G16" s="16">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="15">
-        <v>5</v>
-      </c>
-      <c r="D17" s="15">
-        <v>2</v>
-      </c>
-      <c r="E17" s="15">
-        <v>5</v>
-      </c>
-      <c r="F17" s="15">
-        <v>6</v>
-      </c>
-      <c r="G17" s="16">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="15">
-        <v>6</v>
-      </c>
-      <c r="D18" s="15">
-        <v>5</v>
-      </c>
-      <c r="E18" s="15">
-        <v>6</v>
-      </c>
-      <c r="F18" s="15">
-        <v>7</v>
-      </c>
-      <c r="G18" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="17">
-        <v>6</v>
-      </c>
-      <c r="D19" s="15">
-        <v>1</v>
-      </c>
-      <c r="E19" s="15">
-        <v>5</v>
-      </c>
-      <c r="F19" s="15">
-        <v>8</v>
-      </c>
-      <c r="G19" s="16">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="15">
-        <v>9</v>
-      </c>
-      <c r="D20" s="15">
-        <v>3</v>
-      </c>
-      <c r="E20" s="15">
-        <v>9</v>
-      </c>
-      <c r="F20" s="15">
-        <v>3</v>
-      </c>
-      <c r="G20" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="15">
-        <v>9</v>
-      </c>
-      <c r="D21" s="15">
-        <v>6</v>
-      </c>
-      <c r="E21" s="15">
-        <v>9</v>
-      </c>
-      <c r="F21" s="15">
-        <v>7</v>
-      </c>
-      <c r="G21" s="16">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="15">
-        <v>9</v>
-      </c>
-      <c r="D22" s="15">
-        <v>3</v>
-      </c>
-      <c r="E22" s="15">
-        <v>9</v>
-      </c>
-      <c r="F22" s="15">
-        <v>1</v>
-      </c>
-      <c r="G22" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="15">
-        <v>9</v>
-      </c>
-      <c r="D23" s="15">
-        <v>4</v>
-      </c>
-      <c r="E23" s="15">
-        <v>8</v>
-      </c>
-      <c r="F23" s="15">
-        <v>5</v>
-      </c>
-      <c r="G23" s="16">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="15">
-        <v>10</v>
-      </c>
-      <c r="D24" s="15">
-        <v>5</v>
-      </c>
-      <c r="E24" s="15">
-        <v>10</v>
-      </c>
-      <c r="F24" s="15">
-        <v>3</v>
-      </c>
-      <c r="G24" s="16">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="15">
-        <v>11</v>
-      </c>
-      <c r="D25" s="15">
-        <v>2</v>
-      </c>
-      <c r="E25" s="15">
-        <v>11</v>
-      </c>
-      <c r="F25" s="15">
-        <v>5</v>
-      </c>
-      <c r="G25" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="15">
-        <v>12</v>
-      </c>
-      <c r="D26" s="15">
-        <v>6</v>
-      </c>
-      <c r="E26" s="15">
-        <v>12</v>
-      </c>
-      <c r="F26" s="15">
-        <v>7</v>
-      </c>
-      <c r="G26" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="14" t="s">
+      <c r="D50" s="14">
         <v>28</v>
       </c>
-      <c r="C27" s="15">
-        <v>12</v>
-      </c>
-      <c r="D27" s="15">
-        <v>1</v>
-      </c>
-      <c r="E27" s="15">
-        <v>12</v>
-      </c>
-      <c r="F27" s="15">
-        <v>5</v>
-      </c>
-      <c r="G27" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="15">
-        <v>14</v>
-      </c>
-      <c r="D28" s="15">
-        <v>5</v>
-      </c>
-      <c r="E28" s="15">
-        <v>14</v>
-      </c>
-      <c r="F28" s="15">
-        <v>6</v>
-      </c>
-      <c r="G28" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="14" t="s">
+      <c r="E50" s="14">
+        <v>16</v>
+      </c>
+      <c r="F50" s="14">
         <v>30</v>
       </c>
-      <c r="C29" s="15">
-        <v>14</v>
-      </c>
-      <c r="D29" s="15">
-        <v>8</v>
-      </c>
-      <c r="E29" s="15">
-        <v>14</v>
-      </c>
-      <c r="F29" s="15">
-        <v>2</v>
-      </c>
-      <c r="G29" s="16">
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C30" s="15">
-        <v>14</v>
-      </c>
-      <c r="D30" s="15">
-        <v>7</v>
-      </c>
-      <c r="E30" s="15">
-        <v>14</v>
-      </c>
-      <c r="F30" s="15">
-        <v>3</v>
-      </c>
-      <c r="G30" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" s="15">
-        <v>15</v>
-      </c>
-      <c r="D31" s="15">
-        <v>4</v>
-      </c>
-      <c r="E31" s="15">
-        <v>15</v>
-      </c>
-      <c r="F31" s="15">
-        <v>8</v>
-      </c>
-      <c r="G31" s="16">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" s="15">
-        <v>15</v>
-      </c>
-      <c r="D32" s="15">
-        <v>5</v>
-      </c>
-      <c r="E32" s="15">
-        <v>15</v>
-      </c>
-      <c r="F32" s="15">
-        <v>3</v>
-      </c>
-      <c r="G32" s="16">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" s="15">
-        <v>15</v>
-      </c>
-      <c r="D33" s="15">
-        <v>8</v>
-      </c>
-      <c r="E33" s="15">
-        <v>15</v>
-      </c>
-      <c r="F33" s="15">
-        <v>5</v>
-      </c>
-      <c r="G33" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C34" s="15">
-        <v>16</v>
-      </c>
-      <c r="D34" s="15">
-        <v>28</v>
-      </c>
-      <c r="E34" s="15">
-        <v>16</v>
-      </c>
-      <c r="F34" s="15">
-        <v>30</v>
-      </c>
-      <c r="G34" s="16">
-        <v>0.5</v>
+      <c r="G50" s="15">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:G4"/>
   </mergeCells>
-  <conditionalFormatting sqref="I9:BP34">
+  <conditionalFormatting sqref="I9:BC50">
     <cfRule type="expression" dxfId="9" priority="1">
       <formula>ProzentAbgeschlossen</formula>
     </cfRule>
@@ -1820,12 +2023,12 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B35:BP35">
+  <conditionalFormatting sqref="B51:BC51">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I8:BP8">
+  <conditionalFormatting sqref="I8:BC8">
     <cfRule type="expression" dxfId="0" priority="8">
       <formula>I$8=Ausgewählter_Zeitraum</formula>
     </cfRule>
@@ -1844,15 +2047,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>17</xdr:col>
-                    <xdr:colOff>66675</xdr:colOff>
+                    <xdr:colOff>68580</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:rowOff>30480</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>17</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:col>18</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>257175</xdr:rowOff>
+                    <xdr:rowOff>259080</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>

</xml_diff>

<commit_message>
Test & Gannt fertiggestellt
</commit_message>
<xml_diff>
--- a/documents/projectmanagement/3_Planung/Gantt_Projektplan.xlsx
+++ b/documents/projectmanagement/3_Planung/Gantt_Projektplan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11592"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
   </bookViews>
   <sheets>
     <sheet name="Projekt" sheetId="1" r:id="rId1"/>
@@ -731,15 +731,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>17</xdr:col>
-          <xdr:colOff>68580</xdr:colOff>
+          <xdr:colOff>66675</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>30480</xdr:rowOff>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>18</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>259080</xdr:rowOff>
+          <xdr:rowOff>257175</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1008,24 +1008,24 @@
   </sheetPr>
   <dimension ref="B2:BD50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.77734375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="35.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.21875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.21875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="7.21875" style="7" customWidth="1"/>
-    <col min="8" max="8" width="4.21875" style="1" customWidth="1"/>
-    <col min="9" max="28" width="2.77734375" style="1"/>
+    <col min="1" max="1" width="2.625" customWidth="1"/>
+    <col min="2" max="2" width="35.625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.25" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.25" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="7.25" style="7" customWidth="1"/>
+    <col min="8" max="8" width="4.25" style="1" customWidth="1"/>
+    <col min="9" max="28" width="2.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:56" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:56" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="22" t="s">
         <v>0</v>
       </c>
@@ -1035,7 +1035,7 @@
       <c r="F2" s="22"/>
       <c r="G2" s="22"/>
     </row>
-    <row r="3" spans="2:56" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:56" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
@@ -1084,7 +1084,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
@@ -1097,12 +1097,12 @@
       <c r="AW4" s="1"/>
       <c r="AX4" s="1"/>
     </row>
-    <row r="5" spans="2:56" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:56" x14ac:dyDescent="0.3">
       <c r="AT5" s="1"/>
       <c r="AU5" s="1"/>
       <c r="AV5" s="1"/>
     </row>
-    <row r="6" spans="2:56" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:56" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
         <v>3</v>
@@ -1126,7 +1126,7 @@
       <c r="AU6" s="1"/>
       <c r="AV6" s="1"/>
     </row>
-    <row r="7" spans="2:56" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:56" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1151,7 +1151,7 @@
       </c>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="2:56" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:56" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -1302,7 +1302,7 @@
       </c>
       <c r="BD8" s="1"/>
     </row>
-    <row r="9" spans="2:56" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:56" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
         <v>17</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
         <v>21</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:56" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:56" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="20" t="s">
         <v>25</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:56" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:56" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="21" t="s">
         <v>18</v>
       </c>
@@ -1382,7 +1382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:56" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:56" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="20" t="s">
         <v>49</v>
       </c>
@@ -1402,7 +1402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:56" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:56" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="20" t="s">
         <v>19</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:56" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:56" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="20" t="s">
         <v>23</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:56" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:56" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="20" t="s">
         <v>20</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="20" t="s">
         <v>29</v>
       </c>
@@ -1482,7 +1482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="20" t="s">
         <v>24</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="20" t="s">
         <v>22</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="20" t="s">
         <v>16</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="20" t="s">
         <v>30</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="20" t="s">
         <v>28</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="20" t="s">
         <v>31</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="20" t="s">
         <v>26</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="20" t="s">
         <v>27</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="20" t="s">
         <v>15</v>
       </c>
@@ -1662,7 +1662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="20" t="s">
         <v>32</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="20" t="s">
         <v>33</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="20" t="s">
         <v>34</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="20" t="s">
         <v>35</v>
       </c>
@@ -1742,7 +1742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="20" t="s">
         <v>36</v>
       </c>
@@ -1762,7 +1762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="20" t="s">
         <v>37</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="20" t="s">
         <v>38</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="20" t="s">
         <v>39</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="20" t="s">
         <v>40</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="20" t="s">
         <v>41</v>
       </c>
@@ -1852,13 +1852,17 @@
       <c r="D36" s="14">
         <v>13</v>
       </c>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
+      <c r="E36" s="14">
+        <v>24</v>
+      </c>
+      <c r="F36" s="14">
+        <v>13</v>
+      </c>
       <c r="G36" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="20" t="s">
         <v>42</v>
       </c>
@@ -1868,13 +1872,17 @@
       <c r="D37" s="14">
         <v>3</v>
       </c>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
+      <c r="E37" s="14">
+        <v>24</v>
+      </c>
+      <c r="F37" s="14">
+        <v>3</v>
+      </c>
       <c r="G37" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="20" t="s">
         <v>43</v>
       </c>
@@ -1884,13 +1892,17 @@
       <c r="D38" s="14">
         <v>12</v>
       </c>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
+      <c r="E38" s="14">
+        <v>25</v>
+      </c>
+      <c r="F38" s="14">
+        <v>12</v>
+      </c>
       <c r="G38" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="20" t="s">
         <v>44</v>
       </c>
@@ -1900,13 +1912,17 @@
       <c r="D39" s="14">
         <v>12</v>
       </c>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
+      <c r="E39" s="14">
+        <v>25</v>
+      </c>
+      <c r="F39" s="14">
+        <v>12</v>
+      </c>
       <c r="G39" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="20" t="s">
         <v>45</v>
       </c>
@@ -1916,13 +1932,17 @@
       <c r="D40" s="14">
         <v>12</v>
       </c>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
+      <c r="E40" s="14">
+        <v>25</v>
+      </c>
+      <c r="F40" s="14">
+        <v>12</v>
+      </c>
       <c r="G40" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="20" t="s">
         <v>46</v>
       </c>
@@ -1932,13 +1952,17 @@
       <c r="D41" s="14">
         <v>12</v>
       </c>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
+      <c r="E41" s="14">
+        <v>25</v>
+      </c>
+      <c r="F41" s="14">
+        <v>12</v>
+      </c>
       <c r="G41" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="20" t="s">
         <v>47</v>
       </c>
@@ -1948,13 +1972,17 @@
       <c r="D42" s="14">
         <v>10</v>
       </c>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
+      <c r="E42" s="14">
+        <v>37</v>
+      </c>
+      <c r="F42" s="14">
+        <v>10</v>
+      </c>
       <c r="G42" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="20" t="s">
         <v>55</v>
       </c>
@@ -1964,13 +1992,17 @@
       <c r="D43" s="14">
         <v>3</v>
       </c>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
+      <c r="E43" s="14">
+        <v>37</v>
+      </c>
+      <c r="F43" s="14">
+        <v>3</v>
+      </c>
       <c r="G43" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="20" t="s">
         <v>56</v>
       </c>
@@ -1980,11 +2012,17 @@
       <c r="D44" s="14">
         <v>3</v>
       </c>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="15"/>
-    </row>
-    <row r="45" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E44" s="14">
+        <v>40</v>
+      </c>
+      <c r="F44" s="14">
+        <v>3</v>
+      </c>
+      <c r="G44" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="20" t="s">
         <v>48</v>
       </c>
@@ -1994,13 +2032,17 @@
       <c r="D45" s="14">
         <v>4</v>
       </c>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
+      <c r="E45" s="14">
+        <v>43</v>
+      </c>
+      <c r="F45" s="14">
+        <v>4</v>
+      </c>
       <c r="G45" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="20" t="s">
         <v>50</v>
       </c>
@@ -2010,13 +2052,17 @@
       <c r="D46" s="14">
         <v>1</v>
       </c>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
+      <c r="E46" s="14">
+        <v>47</v>
+      </c>
+      <c r="F46" s="14">
+        <v>1</v>
+      </c>
       <c r="G46" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="20" t="s">
         <v>51</v>
       </c>
@@ -2026,13 +2072,17 @@
       <c r="D47" s="14">
         <v>1</v>
       </c>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
+      <c r="E47" s="14">
+        <v>47</v>
+      </c>
+      <c r="F47" s="14">
+        <v>1</v>
+      </c>
       <c r="G47" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="20" t="s">
         <v>52</v>
       </c>
@@ -2042,13 +2092,17 @@
       <c r="D48" s="14">
         <v>1</v>
       </c>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
+      <c r="E48" s="14">
+        <v>47</v>
+      </c>
+      <c r="F48" s="14">
+        <v>1</v>
+      </c>
       <c r="G48" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="20" t="s">
         <v>53</v>
       </c>
@@ -2058,13 +2112,17 @@
       <c r="D49" s="14">
         <v>1</v>
       </c>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
+      <c r="E49" s="14">
+        <v>47</v>
+      </c>
+      <c r="F49" s="14">
+        <v>1</v>
+      </c>
       <c r="G49" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="20" t="s">
         <v>54</v>
       </c>
@@ -2074,10 +2132,14 @@
       <c r="D50" s="14">
         <v>1</v>
       </c>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
+      <c r="E50" s="14">
+        <v>47</v>
+      </c>
+      <c r="F50" s="14">
+        <v>1</v>
+      </c>
       <c r="G50" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2134,15 +2196,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>17</xdr:col>
-                    <xdr:colOff>68580</xdr:colOff>
+                    <xdr:colOff>66675</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>30480</xdr:rowOff>
+                    <xdr:rowOff>28575</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>18</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>259080</xdr:rowOff>
+                    <xdr:rowOff>257175</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>

</xml_diff>